<commit_message>
Daily purchases excel template
</commit_message>
<xml_diff>
--- a/resources/website/static/edited_file.xlsx
+++ b/resources/website/static/edited_file.xlsx
@@ -1309,7 +1309,7 @@
       <c r="E4" s="42" t="n"/>
       <c r="F4" s="43" t="n"/>
       <c r="G4" s="34">
-        <f>SUM(G5:G8)</f>
+        <f>SUM(G5:G9)</f>
         <v/>
       </c>
       <c r="H4" s="34" t="n"/>
@@ -1318,7 +1318,7 @@
       <c r="K4" s="34" t="n"/>
       <c r="L4" s="34" t="n"/>
       <c r="M4" s="34">
-        <f>SUM(M5:M8)</f>
+        <f>SUM(M5:M9)</f>
         <v/>
       </c>
       <c r="N4" s="34" t="n"/>
@@ -1327,13 +1327,13 @@
       <c r="Q4" s="34" t="n"/>
       <c r="R4" s="34" t="n"/>
       <c r="S4" s="35">
-        <f>SUM(S5:S8)</f>
+        <f>SUM(S5:S9)</f>
         <v/>
       </c>
       <c r="T4" s="34" t="n"/>
       <c r="U4" s="34" t="n"/>
       <c r="V4" s="34">
-        <f>SUM(V5:V8)</f>
+        <f>SUM(V5:V9)</f>
         <v/>
       </c>
       <c r="W4" s="34" t="n"/>
@@ -1342,11 +1342,11 @@
       <c r="Z4" s="34" t="n"/>
       <c r="AA4" s="34" t="n"/>
       <c r="AB4" s="35">
-        <f>SUM(AB5:AB8)</f>
+        <f>SUM(AB5:AB9)</f>
         <v/>
       </c>
       <c r="AC4" s="35">
-        <f>SUM(AC5:AC8)</f>
+        <f>SUM(AC5:AC9)</f>
         <v/>
       </c>
     </row>
@@ -1390,8 +1390,9 @@
       <c r="AB5" t="n">
         <v>1.81</v>
       </c>
-      <c r="AC5" t="n">
-        <v>5.95</v>
+      <c r="AC5">
+        <f>SUM(S5,AB5)</f>
+        <v/>
       </c>
     </row>
     <row r="6">
@@ -1432,8 +1433,9 @@
       <c r="AB6" t="n">
         <v>1.9</v>
       </c>
-      <c r="AC6" t="n">
-        <v>10.9</v>
+      <c r="AC6">
+        <f>SUM(S6,AB6)</f>
+        <v/>
       </c>
     </row>
     <row r="7">
@@ -1476,8 +1478,9 @@
       <c r="AB7" t="n">
         <v>1.81</v>
       </c>
-      <c r="AC7" t="n">
-        <v>1.81</v>
+      <c r="AC7">
+        <f>SUM(S7,AB7)</f>
+        <v/>
       </c>
     </row>
     <row r="8">
@@ -1520,8 +1523,9 @@
       <c r="AB8" t="n">
         <v>1.9</v>
       </c>
-      <c r="AC8" t="n">
-        <v>10.9</v>
+      <c r="AC8">
+        <f>SUM(S8,AB8)</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed unnecessary static files
</commit_message>
<xml_diff>
--- a/resources/website/static/edited_file.xlsx
+++ b/resources/website/static/edited_file.xlsx
@@ -942,7 +942,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC8"/>
+  <dimension ref="A1:AC9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
@@ -1309,7 +1309,7 @@
       <c r="E4" s="42" t="n"/>
       <c r="F4" s="43" t="n"/>
       <c r="G4" s="34">
-        <f>SUM(G5:G9)</f>
+        <f>SUM(G5:G10)</f>
         <v/>
       </c>
       <c r="H4" s="34" t="n"/>
@@ -1318,7 +1318,7 @@
       <c r="K4" s="34" t="n"/>
       <c r="L4" s="34" t="n"/>
       <c r="M4" s="34">
-        <f>SUM(M5:M9)</f>
+        <f>SUM(M5:M10)</f>
         <v/>
       </c>
       <c r="N4" s="34" t="n"/>
@@ -1327,13 +1327,13 @@
       <c r="Q4" s="34" t="n"/>
       <c r="R4" s="34" t="n"/>
       <c r="S4" s="35">
-        <f>SUM(S5:S9)</f>
+        <f>SUM(S5:S10)</f>
         <v/>
       </c>
       <c r="T4" s="34" t="n"/>
       <c r="U4" s="34" t="n"/>
       <c r="V4" s="34">
-        <f>SUM(V5:V9)</f>
+        <f>SUM(V5:V10)</f>
         <v/>
       </c>
       <c r="W4" s="34" t="n"/>
@@ -1342,11 +1342,11 @@
       <c r="Z4" s="34" t="n"/>
       <c r="AA4" s="34" t="n"/>
       <c r="AB4" s="35">
-        <f>SUM(AB5:AB9)</f>
+        <f>SUM(AB5:AB10)</f>
         <v/>
       </c>
       <c r="AC4" s="35">
-        <f>SUM(AC5:AC9)</f>
+        <f>SUM(AC5:AC10)</f>
         <v/>
       </c>
     </row>
@@ -1356,12 +1356,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>12.01.2024</t>
+          <t>16.01.2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>sot</t>
+          <t>2024/01/16</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1379,16 +1379,16 @@
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>23</v>
+        <v>22.1</v>
       </c>
       <c r="S5" t="n">
-        <v>4.14</v>
+        <v>3.98</v>
       </c>
       <c r="V5" t="n">
-        <v>22.6</v>
+        <v>0</v>
       </c>
       <c r="AB5" t="n">
-        <v>1.81</v>
+        <v>0</v>
       </c>
       <c r="AC5">
         <f>SUM(S5,AB5)</f>
@@ -1406,32 +1406,34 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2024-01-12</t>
+          <t>sot</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>KOSMONTE FOODS SHPK</t>
+          <t xml:space="preserve">Magic Ice </t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>810828858</v>
-      </c>
-      <c r="F6" t="inlineStr"/>
+        <v>810379471</v>
+      </c>
+      <c r="F6" t="n">
+        <v>330065898</v>
+      </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="S6" t="n">
-        <v>9</v>
+        <v>4.14</v>
       </c>
       <c r="V6" t="n">
-        <v>23.8</v>
+        <v>22.6</v>
       </c>
       <c r="AB6" t="n">
-        <v>1.9</v>
+        <v>1.81</v>
       </c>
       <c r="AC6">
         <f>SUM(S6,AB6)</f>
@@ -1444,39 +1446,37 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>10.01.2024</t>
+          <t>12.01.2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>neser</t>
+          <t>2024-01-12</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ELKOS SHPK</t>
+          <t>KOSMONTE FOODS SHPK</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>810413584</v>
-      </c>
-      <c r="F7" t="n">
-        <v>330064668</v>
-      </c>
+        <v>810828858</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="S7" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="V7" t="n">
-        <v>22.6</v>
+        <v>23.8</v>
       </c>
       <c r="AB7" t="n">
-        <v>1.81</v>
+        <v>1.9</v>
       </c>
       <c r="AC7">
         <f>SUM(S7,AB7)</f>
@@ -1494,7 +1494,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2024-01-10</t>
+          <t>neser</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1512,19 +1512,64 @@
         <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>23.8</v>
+        <v>22.6</v>
       </c>
       <c r="AB8" t="n">
-        <v>1.9</v>
+        <v>1.81</v>
       </c>
       <c r="AC8">
         <f>SUM(S8,AB8)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>10.01.2024</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2024-01-10</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>ELKOS SHPK</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>810413584</v>
+      </c>
+      <c r="F9" t="n">
+        <v>330064668</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>50</v>
+      </c>
+      <c r="S9" t="n">
+        <v>9</v>
+      </c>
+      <c r="V9" t="n">
+        <v>23.8</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="AC9">
+        <f>SUM(S9,AB9)</f>
         <v/>
       </c>
     </row>

</xml_diff>